<commit_message>
now fix the desc problem at the custom mode
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/OJY.xlsx
+++ b/invoice_gen/TEMPLATE/OJY.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\gen_inv\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\automate invoice\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E16DCC2-378B-4D6B-B91C-229A33465693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB0609E-09CD-423D-9ECA-78F39E73EBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,6 @@
     <sheet name="Packing list" sheetId="9" r:id="rId2"/>
     <sheet name="Invoice" sheetId="12" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Packing list'!$A$13:$B$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$1:$F$37</definedName>
@@ -44,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
   <si>
     <t>SALES CONTRACT</t>
   </si>
@@ -907,6 +904,21 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -915,36 +927,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -962,17 +944,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1287,31 +1284,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Contract"/>
-      <sheetName val="Packing list"/>
-      <sheetName val="Invoice OJY24001"/>
-      <sheetName val="Invoice OJY24001 SIGN"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="10">
-          <cell r="F10" t="str">
-            <v>Delivery term:</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1573,7 +1545,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1589,33 +1561,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45.95" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
     </row>
     <row r="2" spans="1:6" customFormat="1" ht="27" customHeight="1">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
     </row>
     <row r="3" spans="1:6" s="40" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="45"/>
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="71"/>
+      <c r="E3" s="76"/>
       <c r="F3" s="47" t="s">
         <v>70</v>
       </c>
@@ -1624,10 +1596,10 @@
       <c r="A4" s="48"/>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="71"/>
+      <c r="E4" s="76"/>
       <c r="F4" s="49" t="s">
         <v>72</v>
       </c>
@@ -1636,13 +1608,13 @@
       <c r="A5" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
     </row>
     <row r="6" spans="1:6" s="40" customFormat="1" ht="21.95" customHeight="1">
       <c r="A6" s="52"/>
@@ -1678,65 +1650,65 @@
       <c r="A9" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
     </row>
     <row r="10" spans="1:6" s="40" customFormat="1" ht="27.95" customHeight="1">
       <c r="A10" s="50"/>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
     </row>
     <row r="11" spans="1:6" s="40" customFormat="1" ht="18.95" customHeight="1">
       <c r="A11" s="50"/>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
     </row>
     <row r="12" spans="1:6" s="40" customFormat="1" ht="18.95" customHeight="1">
       <c r="A12" s="50"/>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
     </row>
     <row r="13" spans="1:6" s="40" customFormat="1" ht="21.95" customHeight="1">
       <c r="A13" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
     </row>
     <row r="14" spans="1:6" s="41" customFormat="1" ht="39" customHeight="1">
       <c r="A14" s="55"/>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
     </row>
     <row r="15" spans="1:6" s="41" customFormat="1" ht="24.95" customHeight="1">
       <c r="A15" s="55" t="s">
@@ -1771,34 +1743,34 @@
       <c r="F17" s="55"/>
     </row>
     <row r="18" spans="1:7" s="40" customFormat="1" ht="30.95" customHeight="1">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
     </row>
     <row r="19" spans="1:7" s="40" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="56"/>
@@ -1874,11 +1846,11 @@
       </c>
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>
-      <c r="D28" s="74" t="s">
+      <c r="D28" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:7" s="42" customFormat="1" ht="41.1" customHeight="1">
       <c r="A29" s="50" t="s">
@@ -1886,11 +1858,11 @@
       </c>
       <c r="B29" s="50"/>
       <c r="C29" s="50"/>
-      <c r="D29" s="74" t="s">
+      <c r="D29" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
     </row>
     <row r="30" spans="1:7" s="42" customFormat="1" ht="29.1" customHeight="1">
       <c r="A30" s="50" t="s">
@@ -1898,11 +1870,11 @@
       </c>
       <c r="B30" s="50"/>
       <c r="C30" s="50"/>
-      <c r="D30" s="75" t="s">
+      <c r="D30" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
     </row>
     <row r="31" spans="1:7" s="42" customFormat="1" ht="29.1" customHeight="1">
       <c r="A31" s="50" t="s">
@@ -1938,24 +1910,24 @@
       <c r="F33" s="52"/>
     </row>
     <row r="34" spans="1:6" s="43" customFormat="1" ht="57" customHeight="1">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="76"/>
+      <c r="B34" s="71"/>
       <c r="C34" s="60"/>
       <c r="D34" s="56"/>
-      <c r="E34" s="76" t="s">
+      <c r="E34" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="76"/>
+      <c r="F34" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B5:F5"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A19:F19"/>
@@ -1965,11 +1937,11 @@
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:F13"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="E34:F34"/>
   </mergeCells>
   <pageMargins left="0.35763888888888901" right="0.35763888888888901" top="0.80277777777777803" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="61" orientation="portrait" r:id="rId1"/>
@@ -1988,7 +1960,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="27" customHeight="1"/>
@@ -2011,92 +1983,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
       <c r="J3" s="33"/>
       <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
       <c r="J4" s="33"/>
       <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" ht="27" customHeight="1">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="27" customHeight="1">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="36"/>
       <c r="K6" s="36"/>
     </row>
@@ -2148,9 +2120,8 @@
         <v>46</v>
       </c>
       <c r="F10" s="18"/>
-      <c r="H10" s="67" t="str">
-        <f>'[1]Invoice OJY24001'!F10</f>
-        <v>Delivery term:</v>
+      <c r="H10" s="67" t="s">
+        <v>60</v>
       </c>
       <c r="I10" s="68" t="s">
         <v>47</v>
@@ -2271,14 +2242,14 @@
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
       <c r="I21" s="39"/>
-      <c r="L21" s="82"/>
+      <c r="L21" s="77"/>
     </row>
     <row r="22" spans="1:12" ht="27" customHeight="1">
-      <c r="A22" s="85" t="s">
+      <c r="A22" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="85"/>
-      <c r="C22" s="85"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="31"/>
@@ -2287,38 +2258,38 @@
       <c r="I22" s="11"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
-      <c r="L22" s="82"/>
+      <c r="L22" s="77"/>
     </row>
     <row r="23" spans="1:12" ht="27" customHeight="1">
       <c r="A23" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="81"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:12" ht="27" customHeight="1">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
       <c r="J24" s="33"/>
       <c r="K24" s="33"/>
       <c r="L24" s="38"/>
@@ -2374,8 +2345,8 @@
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
-      <c r="J30" s="83"/>
-      <c r="K30" s="83"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="78"/>
     </row>
     <row r="31" spans="1:12" ht="27" customHeight="1">
       <c r="F31" s="18"/>
@@ -2386,17 +2357,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="N22:N34">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -2416,8 +2387,8 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A3" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -2438,70 +2409,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="1:7" ht="39" customHeight="1">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="F7" s="5" t="s">
@@ -2624,11 +2595,11 @@
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="42" customHeight="1">
-      <c r="A22" s="85" t="s">
+      <c r="A22" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="85"/>
-      <c r="C22" s="85"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="2"/>
       <c r="G22" s="11"/>
     </row>
@@ -2636,47 +2607,47 @@
       <c r="A23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="90" t="s">
+      <c r="B23" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="90"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" ht="42" customHeight="1">
-      <c r="A24" s="91" t="s">
+      <c r="A24" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A25" s="89" t="s">
+      <c r="A25" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="89"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="89"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
-      <c r="A26" s="89" t="s">
+      <c r="A26" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="89"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="42" customHeight="1">
       <c r="F27" s="11" t="s">
@@ -2718,17 +2689,17 @@
     <row r="61" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="J22:J33">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>

</xml_diff>